<commit_message>
Se añadió la tabla de tiempos
</commit_message>
<xml_diff>
--- a/docs/Resultados.xlsx
+++ b/docs/Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Programacion\5to Semestre\TC2017-PF-Otono-2019-pasplis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2669127C-3FF2-4792-B70A-1FEDC901F5E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1933A1-FD67-4F05-8D7B-25C385B693B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FD59AB03-1603-4A82-8D1C-48D5465E0630}"/>
   </bookViews>
@@ -1770,6 +1770,1039 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Medidas en general</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$5:$D$5,Hoja1!$H$5:$I$5,Hoja1!$M$5:$N$5,Hoja1!$R$5:$S$5)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37459999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61329999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1500000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$6:$D$6,Hoja1!$H$6:$I$6,Hoja1!$M$6:$N$6,Hoja1!$R$6:$S$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.54459999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1532</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.686999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21310000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$7:$D$7,Hoja1!$H$7:$I$7,Hoja1!$M$7:$N$7,Hoja1!$R$7:$S$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.62870000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1883</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.571</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1883</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9689999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1883</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1883</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$8:$D$8,Hoja1!$H$8:$I$8,Hoja1!$M$8:$N$8,Hoja1!$R$8:$S$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>30.492000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4455</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2894999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0804999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.38250000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$9:$D$9,Hoja1!$H$9:$I$9,Hoja1!$M$9:$N$9,Hoja1!$R$9:$S$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.63780000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51290000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7046999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51290000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8294999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51290000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.51290000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$10:$D$10,Hoja1!$H$10:$I$10,Hoja1!$M$10:$N$10,Hoja1!$R$10:$S$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0478000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8120000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5563</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9947999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5563</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5563</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$11:$D$11,Hoja1!$H$11:$I$11,Hoja1!$M$11:$N$11,Hoja1!$R$11:$S$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.4671000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82979999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82979999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1525999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82979999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.571999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82979999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$12:$D$12,Hoja1!$H$12:$I$12,Hoja1!$M$12:$N$12,Hoja1!$R$12:$S$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.0647000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7372999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.749000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7372999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.566000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7372999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7372999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$C$4:$D$4,Hoja1!$H$4:$I$4,Hoja1!$M$4:$N$4,Hoja1!$R$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Paralelo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$13:$D$13,Hoja1!$H$13:$I$13,Hoja1!$M$13:$N$13,Hoja1!$R$13:$S$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.4314999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.896000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1796</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.090999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1796</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.503</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-BD8D-4A90-9AB8-4031AE8ECCFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="588338784"/>
+        <c:axId val="588335832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="588338784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588335832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="588335832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588338784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1930,6 +2963,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3962,6 +5035,511 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4106,16 +5684,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4135,6 +5713,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E54464B-952D-40BF-B90D-6EAE033FA660}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4442,8 +6056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8979AC-E86F-4216-A4EE-5308FBA94DAF}">
   <dimension ref="B4:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>